<commit_message>
REport SAles oke. done.
</commit_message>
<xml_diff>
--- a/rpt/nested-sales.xlsx
+++ b/rpt/nested-sales.xlsx
@@ -168,6 +168,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="G8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Customer</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G11" authorId="0">
       <text>
         <r>
@@ -177,7 +190,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Quantity</t>
+          <t xml:space="preserve">SellQuantity</t>
         </r>
       </text>
     </comment>
@@ -190,7 +203,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Quantity</t>
+          <t xml:space="preserve">SellQuantity</t>
         </r>
       </text>
     </comment>
@@ -251,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t xml:space="preserve">Sales Report Category with Sub-Category</t>
   </si>
@@ -281,6 +294,12 @@
   </si>
   <si>
     <t xml:space="preserve">MENU PAKET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Agoes goes</t>
   </si>
   <si>
     <t xml:space="preserve">Sub-Category :</t>
@@ -483,7 +502,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -615,7 +634,7 @@
   <dimension ref="A2:J14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -701,17 +720,22 @@
       <c r="D8" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="F8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,36 +743,36 @@
         <v>2</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F11" s="13" t="n">
         <v>20</v>
@@ -757,25 +781,25 @@
         <v>100</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I11" s="13" t="n">
         <f aca="false">G11*F11</f>
         <v>2000</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F12" s="17" t="n">
         <v>0.2</v>
@@ -784,14 +808,14 @@
         <v>100</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I12" s="18" t="n">
         <f aca="false">G12*F12</f>
         <v>20</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>